<commit_message>
removed wrong date from time only variables
</commit_message>
<xml_diff>
--- a/config/config.xlsx
+++ b/config/config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dom/Repos/github.com/DominikFin/nlp-satisfaction/config/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50225900-F69E-B948-AAFE-24987B33599D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B2D0358-FCFB-F34C-9D63-16094E5D797C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="24140" yWindow="8780" windowWidth="33600" windowHeight="19220" xr2:uid="{200F5F93-4F8B-1441-AC51-6C611B6C2579}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="18800" xr2:uid="{200F5F93-4F8B-1441-AC51-6C611B6C2579}"/>
   </bookViews>
   <sheets>
     <sheet name="fragecodes" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="77">
   <si>
     <t>wime_unzuf_sf_txt</t>
   </si>
@@ -268,6 +268,9 @@
   </si>
   <si>
     <t>Anzahl Einladungen</t>
+  </si>
+  <si>
+    <t>time</t>
   </si>
 </sst>
 </file>
@@ -304,12 +307,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -324,11 +333,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -646,7 +656,7 @@
   <dimension ref="A1:C42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E27" sqref="E27"/>
+      <selection activeCell="C37" sqref="C37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -957,7 +967,7 @@
         <v>24</v>
       </c>
       <c r="B28" t="s">
-        <v>62</v>
+        <v>76</v>
       </c>
       <c r="C28" t="s">
         <v>70</v>
@@ -968,7 +978,7 @@
         <v>25</v>
       </c>
       <c r="B29" t="s">
-        <v>62</v>
+        <v>76</v>
       </c>
       <c r="C29" t="s">
         <v>70</v>
@@ -1034,7 +1044,7 @@
         <v>31</v>
       </c>
       <c r="B35" t="s">
-        <v>62</v>
+        <v>76</v>
       </c>
       <c r="C35" t="s">
         <v>70</v>
@@ -1045,7 +1055,7 @@
         <v>32</v>
       </c>
       <c r="B36" t="s">
-        <v>62</v>
+        <v>76</v>
       </c>
       <c r="C36" t="s">
         <v>70</v>
@@ -1384,8 +1394,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C76DEDB6-88B8-E048-9543-65DF58472E86}">
   <dimension ref="A1:E49"/>
   <sheetViews>
-    <sheetView topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="C27" sqref="C27"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="B49" sqref="B49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1770,9 +1780,12 @@
         <v>117247</v>
       </c>
     </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A49" s="3">
         <v>44896</v>
+      </c>
+      <c r="B49" s="4">
+        <v>80000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>